<commit_message>
Mejoras en el motor de R
</commit_message>
<xml_diff>
--- a/motorR/4098796/vecinos_ofertas_nuevas.xlsx
+++ b/motorR/4098796/vecinos_ofertas_nuevas.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="43">
   <si>
     <t xml:space="preserve">job_id</t>
   </si>
@@ -20,34 +20,127 @@
     <t xml:space="preserve">vecinos</t>
   </si>
   <si>
+    <t xml:space="preserve">56</t>
+  </si>
+  <si>
+    <t xml:space="preserve">64</t>
+  </si>
+  <si>
+    <t xml:space="preserve">17</t>
+  </si>
+  <si>
+    <t xml:space="preserve">66</t>
+  </si>
+  <si>
+    <t xml:space="preserve">26</t>
+  </si>
+  <si>
+    <t xml:space="preserve">36</t>
+  </si>
+  <si>
+    <t xml:space="preserve">16</t>
+  </si>
+  <si>
+    <t xml:space="preserve">76</t>
+  </si>
+  <si>
+    <t xml:space="preserve">24</t>
+  </si>
+  <si>
+    <t xml:space="preserve">80</t>
+  </si>
+  <si>
+    <t xml:space="preserve">55</t>
+  </si>
+  <si>
+    <t xml:space="preserve">68</t>
+  </si>
+  <si>
+    <t xml:space="preserve">19</t>
+  </si>
+  <si>
+    <t xml:space="preserve">54</t>
+  </si>
+  <si>
+    <t xml:space="preserve">33</t>
+  </si>
+  <si>
+    <t xml:space="preserve">78</t>
+  </si>
+  <si>
+    <t xml:space="preserve">22</t>
+  </si>
+  <si>
     <t xml:space="preserve">50</t>
   </si>
   <si>
-    <t xml:space="preserve">2</t>
+    <t xml:space="preserve">29</t>
+  </si>
+  <si>
+    <t xml:space="preserve">67</t>
+  </si>
+  <si>
+    <t xml:space="preserve">63</t>
+  </si>
+  <si>
+    <t xml:space="preserve">74</t>
+  </si>
+  <si>
+    <t xml:space="preserve">8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">42</t>
+  </si>
+  <si>
+    <t xml:space="preserve">79</t>
+  </si>
+  <si>
+    <t xml:space="preserve">14</t>
   </si>
   <si>
     <t xml:space="preserve">49</t>
   </si>
   <si>
+    <t xml:space="preserve">27</t>
+  </si>
+  <si>
+    <t xml:space="preserve">41</t>
+  </si>
+  <si>
+    <t xml:space="preserve">60</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5</t>
+  </si>
+  <si>
     <t xml:space="preserve">72</t>
   </si>
   <si>
-    <t xml:space="preserve">63</t>
-  </si>
-  <si>
-    <t xml:space="preserve">11</t>
-  </si>
-  <si>
-    <t xml:space="preserve">57</t>
-  </si>
-  <si>
-    <t xml:space="preserve">16</t>
-  </si>
-  <si>
-    <t xml:space="preserve">55</t>
-  </si>
-  <si>
-    <t xml:space="preserve">23</t>
+    <t xml:space="preserve">30</t>
+  </si>
+  <si>
+    <t xml:space="preserve">13</t>
+  </si>
+  <si>
+    <t xml:space="preserve">44</t>
+  </si>
+  <si>
+    <t xml:space="preserve">51</t>
+  </si>
+  <si>
+    <t xml:space="preserve">59</t>
+  </si>
+  <si>
+    <t xml:space="preserve">25</t>
+  </si>
+  <si>
+    <t xml:space="preserve">46</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">28</t>
   </si>
 </sst>
 </file>
@@ -397,7 +490,7 @@
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B3" t="s">
         <v>3</v>
@@ -405,7 +498,7 @@
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="B4" t="s">
         <v>4</v>
@@ -413,7 +506,7 @@
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="B5" t="s">
         <v>5</v>
@@ -421,7 +514,7 @@
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>71</v>
+        <v>75</v>
       </c>
       <c r="B6" t="s">
         <v>6</v>
@@ -429,7 +522,7 @@
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="B7" t="s">
         <v>7</v>
@@ -437,7 +530,7 @@
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>71</v>
+        <v>77</v>
       </c>
       <c r="B8" t="s">
         <v>8</v>
@@ -445,7 +538,7 @@
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>73</v>
+        <v>78</v>
       </c>
       <c r="B9" t="s">
         <v>9</v>
@@ -453,7 +546,7 @@
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>71</v>
+        <v>79</v>
       </c>
       <c r="B10" t="s">
         <v>10</v>
@@ -461,10 +554,330 @@
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>73</v>
+        <v>80</v>
       </c>
       <c r="B11" t="s">
         <v>11</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>71</v>
+      </c>
+      <c r="B12" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="n">
+        <v>72</v>
+      </c>
+      <c r="B13" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="n">
+        <v>73</v>
+      </c>
+      <c r="B14" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="n">
+        <v>74</v>
+      </c>
+      <c r="B15" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="n">
+        <v>75</v>
+      </c>
+      <c r="B16" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="n">
+        <v>76</v>
+      </c>
+      <c r="B17" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="n">
+        <v>77</v>
+      </c>
+      <c r="B18" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="n">
+        <v>78</v>
+      </c>
+      <c r="B19" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="n">
+        <v>79</v>
+      </c>
+      <c r="B20" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="n">
+        <v>80</v>
+      </c>
+      <c r="B21" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="n">
+        <v>71</v>
+      </c>
+      <c r="B22" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="n">
+        <v>72</v>
+      </c>
+      <c r="B23" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="n">
+        <v>73</v>
+      </c>
+      <c r="B24" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="n">
+        <v>74</v>
+      </c>
+      <c r="B25" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="n">
+        <v>75</v>
+      </c>
+      <c r="B26" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="n">
+        <v>76</v>
+      </c>
+      <c r="B27" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="n">
+        <v>77</v>
+      </c>
+      <c r="B28" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="n">
+        <v>78</v>
+      </c>
+      <c r="B29" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="n">
+        <v>79</v>
+      </c>
+      <c r="B30" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="n">
+        <v>80</v>
+      </c>
+      <c r="B31" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="n">
+        <v>71</v>
+      </c>
+      <c r="B32" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="n">
+        <v>72</v>
+      </c>
+      <c r="B33" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="n">
+        <v>73</v>
+      </c>
+      <c r="B34" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="n">
+        <v>74</v>
+      </c>
+      <c r="B35" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="n">
+        <v>75</v>
+      </c>
+      <c r="B36" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="n">
+        <v>76</v>
+      </c>
+      <c r="B37" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="n">
+        <v>77</v>
+      </c>
+      <c r="B38" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="n">
+        <v>78</v>
+      </c>
+      <c r="B39" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="n">
+        <v>79</v>
+      </c>
+      <c r="B40" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="n">
+        <v>80</v>
+      </c>
+      <c r="B41" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="n">
+        <v>71</v>
+      </c>
+      <c r="B42" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="n">
+        <v>72</v>
+      </c>
+      <c r="B43" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="n">
+        <v>73</v>
+      </c>
+      <c r="B44" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="n">
+        <v>74</v>
+      </c>
+      <c r="B45" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="n">
+        <v>75</v>
+      </c>
+      <c r="B46" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="n">
+        <v>76</v>
+      </c>
+      <c r="B47" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="n">
+        <v>77</v>
+      </c>
+      <c r="B48" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="n">
+        <v>78</v>
+      </c>
+      <c r="B49" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="n">
+        <v>79</v>
+      </c>
+      <c r="B50" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="n">
+        <v>80</v>
+      </c>
+      <c r="B51" t="s">
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>